<commit_message>
Mixer1: BOM - wip
</commit_message>
<xml_diff>
--- a/modules/Mixer1/Mixer1-BOM.xlsx
+++ b/modules/Mixer1/Mixer1-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Mixer1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{67C8148B-B567-4004-8349-4F1142967499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BDF432-86A1-4B2E-8C7E-55F6B643AA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="915" windowWidth="19380" windowHeight="11820"/>
+    <workbookView xWindow="4365" yWindow="915" windowWidth="19380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixer1-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -574,7 +587,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1420,11 +1433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,9 +1653,12 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -1718,9 +1734,12 @@
       <c r="B7">
         <v>2</v>
       </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Mixer1: BOM - done
</commit_message>
<xml_diff>
--- a/modules/Mixer1/Mixer1-BOM.xlsx
+++ b/modules/Mixer1/Mixer1-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Mixer1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D98739-6771-4478-900E-731FE7D6A8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B364F43C-690F-4B61-B2FD-E72EC132FB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4365" yWindow="915" windowWidth="19380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,9 +2040,12 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>120</v>

</xml_diff>